<commit_message>
chore: Update last_date.txt and add new day_data
This commit updates the last_date.txt file to reflect the new deadline and adds a new day_data file for August 30, 2024.
</commit_message>
<xml_diff>
--- a/month_data/August.xlsx
+++ b/month_data/August.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,12 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>06.7</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
         </is>
       </c>
     </row>
@@ -568,6 +573,9 @@
       <c r="P2" t="n">
         <v>1</v>
       </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -622,6 +630,9 @@
       <c r="P3" t="n">
         <v>0</v>
       </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -676,6 +687,9 @@
       <c r="P4" t="n">
         <v>0</v>
       </c>
+      <c r="Q4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -730,6 +744,9 @@
       <c r="P5" t="n">
         <v>0</v>
       </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -784,6 +801,9 @@
       <c r="P6" t="n">
         <v>0</v>
       </c>
+      <c r="Q6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -838,6 +858,9 @@
       <c r="P7" t="n">
         <v>0</v>
       </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -892,6 +915,9 @@
       <c r="P8" t="n">
         <v>0</v>
       </c>
+      <c r="Q8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -946,6 +972,9 @@
       <c r="P9" t="n">
         <v>0</v>
       </c>
+      <c r="Q9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1000,6 +1029,9 @@
       <c r="P10" t="n">
         <v>0</v>
       </c>
+      <c r="Q10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1054,6 +1086,9 @@
       <c r="P11" t="n">
         <v>0</v>
       </c>
+      <c r="Q11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1108,6 +1143,9 @@
       <c r="P12" t="n">
         <v>0</v>
       </c>
+      <c r="Q12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1162,6 +1200,9 @@
       <c r="P13" t="n">
         <v>0</v>
       </c>
+      <c r="Q13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1216,6 +1257,9 @@
       <c r="P14" t="n">
         <v>0</v>
       </c>
+      <c r="Q14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1270,6 +1314,9 @@
       <c r="P15" t="n">
         <v>0</v>
       </c>
+      <c r="Q15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1324,6 +1371,9 @@
       <c r="P16" t="n">
         <v>0</v>
       </c>
+      <c r="Q16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1378,6 +1428,9 @@
       <c r="P17" t="n">
         <v>0</v>
       </c>
+      <c r="Q17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1432,6 +1485,9 @@
       <c r="P18" t="n">
         <v>0</v>
       </c>
+      <c r="Q18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1486,6 +1542,9 @@
       <c r="P19" t="n">
         <v>0</v>
       </c>
+      <c r="Q19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1540,6 +1599,9 @@
       <c r="P20" t="n">
         <v>0</v>
       </c>
+      <c r="Q20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1594,6 +1656,9 @@
       <c r="P21" t="n">
         <v>0</v>
       </c>
+      <c r="Q21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1646,6 +1711,9 @@
         <v>0</v>
       </c>
       <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>